<commit_message>
add simulation results for rollout
</commit_message>
<xml_diff>
--- a/Final Project/simulation.xlsx
+++ b/Final Project/simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgy/Downloads/AI_Proj/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51E5FCF-BA53-514A-91BD-9E34D87D49C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E19FB9-4114-974E-AF34-FF10980C2C38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CB718146-76ED-6B4B-ABE4-D20C3144D41F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CB718146-76ED-6B4B-ABE4-D20C3144D41F}"/>
   </bookViews>
   <sheets>
     <sheet name="hyper" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>tme in sec</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>mcts</t>
-  </si>
-  <si>
-    <t>expectimax</t>
   </si>
   <si>
     <t>algo</t>
@@ -80,10 +77,40 @@
     <t>std</t>
   </si>
   <si>
-    <t>MCTS</t>
+    <t>avg time</t>
   </si>
   <si>
-    <t>avg time</t>
+    <t>MCTS_default</t>
+  </si>
+  <si>
+    <t>rollout</t>
+  </si>
+  <si>
+    <t>rollout_default</t>
+  </si>
+  <si>
+    <t>2.2 GHz Intel Core i7</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>16 GB 1600 MHz DDR3</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>Intel Iris Pro 1536 MB</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>rollout_smooth</t>
+  </si>
+  <si>
+    <t>rollout_depth5</t>
   </si>
 </sst>
 </file>
@@ -450,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4803BA00-13C4-D94B-9AED-D7BFB6F44303}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -464,38 +491,47 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,8 +559,14 @@
       <c r="I2">
         <v>6698</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>12948</v>
+      </c>
+      <c r="K2">
+        <v>15214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -551,6 +593,36 @@
       </c>
       <c r="I3">
         <v>100</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -560,9 +632,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496C838B-E0FA-174D-B6C2-D799DE97087C}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -574,38 +648,43 @@
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1012</v>
       </c>
@@ -630,8 +709,14 @@
       <c r="H2" s="1">
         <v>1908</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" s="1">
+        <v>5380</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3028</v>
       </c>
@@ -656,8 +741,14 @@
       <c r="H3">
         <v>1028</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>5568</v>
+      </c>
+      <c r="J3">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1120</v>
       </c>
@@ -682,8 +773,14 @@
       <c r="H4">
         <v>3132</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>6884</v>
+      </c>
+      <c r="J4">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1132</v>
       </c>
@@ -708,8 +805,14 @@
       <c r="H5">
         <v>1272</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>6560</v>
+      </c>
+      <c r="J5">
+        <v>2916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1460</v>
       </c>
@@ -734,8 +837,14 @@
       <c r="H6">
         <v>2452</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>3288</v>
+      </c>
+      <c r="J6">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1456</v>
       </c>
@@ -760,8 +869,14 @@
       <c r="H7">
         <v>3576</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>1056</v>
+      </c>
+      <c r="J7">
+        <v>5572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>616</v>
       </c>
@@ -786,8 +901,14 @@
       <c r="H8">
         <v>2012</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>1340</v>
+      </c>
+      <c r="J8">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1412</v>
       </c>
@@ -812,8 +933,14 @@
       <c r="H9">
         <v>1776</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>3616</v>
+      </c>
+      <c r="J9">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1440</v>
       </c>
@@ -838,8 +965,14 @@
       <c r="H10">
         <v>1548</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>11464</v>
+      </c>
+      <c r="J10">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1332</v>
       </c>
@@ -864,8 +997,14 @@
       <c r="H11">
         <v>1824</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>6328</v>
+      </c>
+      <c r="J11">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1120</v>
       </c>
@@ -890,8 +1029,14 @@
       <c r="H12">
         <v>4932</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>5348</v>
+      </c>
+      <c r="J12">
+        <v>6424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>820</v>
       </c>
@@ -916,8 +1061,14 @@
       <c r="H13">
         <v>1740</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>1352</v>
+      </c>
+      <c r="J13">
+        <v>5264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1088</v>
       </c>
@@ -942,8 +1093,14 @@
       <c r="H14">
         <v>540</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>4484</v>
+      </c>
+      <c r="J14">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1276</v>
       </c>
@@ -968,8 +1125,14 @@
       <c r="H15">
         <v>1540</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>1180</v>
+      </c>
+      <c r="J15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>484</v>
       </c>
@@ -994,8 +1157,14 @@
       <c r="H16">
         <v>3380</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>6596</v>
+      </c>
+      <c r="J16">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>732</v>
       </c>
@@ -1020,8 +1189,14 @@
       <c r="H17">
         <v>3576</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>4880</v>
+      </c>
+      <c r="J17">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1316</v>
       </c>
@@ -1046,8 +1221,14 @@
       <c r="H18">
         <v>3420</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>2280</v>
+      </c>
+      <c r="J18">
+        <v>5072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1132</v>
       </c>
@@ -1072,8 +1253,14 @@
       <c r="H19">
         <v>3164</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>1404</v>
+      </c>
+      <c r="J19">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>796</v>
       </c>
@@ -1098,8 +1285,14 @@
       <c r="H20">
         <v>2560</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>6792</v>
+      </c>
+      <c r="J20">
+        <v>3488</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1312</v>
       </c>
@@ -1124,8 +1317,14 @@
       <c r="H21">
         <v>6364</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>2680</v>
+      </c>
+      <c r="J21">
+        <v>6028</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>748</v>
       </c>
@@ -1150,8 +1349,14 @@
       <c r="H22">
         <v>2264</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>3476</v>
+      </c>
+      <c r="J22">
+        <v>5440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1332</v>
       </c>
@@ -1176,8 +1381,14 @@
       <c r="H23">
         <v>2628</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>2432</v>
+      </c>
+      <c r="J23">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2060</v>
       </c>
@@ -1202,8 +1413,14 @@
       <c r="H24">
         <v>1436</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>5988</v>
+      </c>
+      <c r="J24">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>896</v>
       </c>
@@ -1228,8 +1445,14 @@
       <c r="H25">
         <v>3112</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>2452</v>
+      </c>
+      <c r="J25">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>156</v>
       </c>
@@ -1254,8 +1477,14 @@
       <c r="H26">
         <v>1620</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>6276</v>
+      </c>
+      <c r="J26">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1448</v>
       </c>
@@ -1280,8 +1509,14 @@
       <c r="H27">
         <v>1368</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>7112</v>
+      </c>
+      <c r="J27">
+        <v>6204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>676</v>
       </c>
@@ -1306,8 +1541,14 @@
       <c r="H28">
         <v>4728</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>1264</v>
+      </c>
+      <c r="J28">
+        <v>2692</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1120</v>
       </c>
@@ -1332,8 +1573,14 @@
       <c r="H29">
         <v>2296</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>4940</v>
+      </c>
+      <c r="J29">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1112</v>
       </c>
@@ -1358,8 +1605,14 @@
       <c r="H30">
         <v>1512</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>7072</v>
+      </c>
+      <c r="J30">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>460</v>
       </c>
@@ -1384,8 +1637,14 @@
       <c r="H31">
         <v>3036</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>1352</v>
+      </c>
+      <c r="J31">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>684</v>
       </c>
@@ -1410,8 +1669,14 @@
       <c r="H32">
         <v>1176</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>5312</v>
+      </c>
+      <c r="J32">
+        <v>4944</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1008</v>
       </c>
@@ -1436,8 +1701,14 @@
       <c r="H33">
         <v>2280</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>1552</v>
+      </c>
+      <c r="J33">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>808</v>
       </c>
@@ -1462,8 +1733,14 @@
       <c r="H34">
         <v>4616</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <v>1172</v>
+      </c>
+      <c r="J34">
+        <v>5416</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1052</v>
       </c>
@@ -1488,8 +1765,14 @@
       <c r="H35">
         <v>3392</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>7380</v>
+      </c>
+      <c r="J35">
+        <v>6284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1388</v>
       </c>
@@ -1514,8 +1797,14 @@
       <c r="H36">
         <v>2308</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>6356</v>
+      </c>
+      <c r="J36">
+        <v>4084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>564</v>
       </c>
@@ -1540,8 +1829,14 @@
       <c r="H37">
         <v>2624</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37">
+        <v>5612</v>
+      </c>
+      <c r="J37">
+        <v>7188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1080</v>
       </c>
@@ -1566,8 +1861,14 @@
       <c r="H38">
         <v>2496</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <v>3124</v>
+      </c>
+      <c r="J38">
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>632</v>
       </c>
@@ -1592,8 +1893,14 @@
       <c r="H39">
         <v>3104</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <v>1108</v>
+      </c>
+      <c r="J39">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>128</v>
       </c>
@@ -1618,8 +1925,14 @@
       <c r="H40">
         <v>1256</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40">
+        <v>3640</v>
+      </c>
+      <c r="J40">
+        <v>5228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1228</v>
       </c>
@@ -1644,8 +1957,14 @@
       <c r="H41">
         <v>2484</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <v>4940</v>
+      </c>
+      <c r="J41">
+        <v>6864</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>820</v>
       </c>
@@ -1670,8 +1989,14 @@
       <c r="H42">
         <v>156</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42">
+        <v>1308</v>
+      </c>
+      <c r="J42">
+        <v>4944</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2968</v>
       </c>
@@ -1696,8 +2021,14 @@
       <c r="H43">
         <v>5296</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43">
+        <v>6328</v>
+      </c>
+      <c r="J43">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2380</v>
       </c>
@@ -1722,8 +2053,14 @@
       <c r="H44">
         <v>2188</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44">
+        <v>3232</v>
+      </c>
+      <c r="J44">
+        <v>5628</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>992</v>
       </c>
@@ -1748,8 +2085,14 @@
       <c r="H45">
         <v>1676</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45">
+        <v>1428</v>
+      </c>
+      <c r="J45">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>864</v>
       </c>
@@ -1774,8 +2117,14 @@
       <c r="H46">
         <v>1604</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <v>1612</v>
+      </c>
+      <c r="J46">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>704</v>
       </c>
@@ -1800,8 +2149,14 @@
       <c r="H47">
         <v>6804</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47">
+        <v>2448</v>
+      </c>
+      <c r="J47">
+        <v>6172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1260</v>
       </c>
@@ -1826,8 +2181,14 @@
       <c r="H48">
         <v>3272</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <v>5668</v>
+      </c>
+      <c r="J48">
+        <v>2936</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1432</v>
       </c>
@@ -1852,8 +2213,14 @@
       <c r="H49">
         <v>3500</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>5572</v>
+      </c>
+      <c r="J49">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>644</v>
       </c>
@@ -1878,8 +2245,14 @@
       <c r="H50">
         <v>724</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <v>6696</v>
+      </c>
+      <c r="J50">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1204</v>
       </c>
@@ -1904,8 +2277,14 @@
       <c r="H51">
         <v>1444</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <v>3384</v>
+      </c>
+      <c r="J51">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1332</v>
       </c>
@@ -1930,8 +2309,14 @@
       <c r="H52">
         <v>636</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <v>2836</v>
+      </c>
+      <c r="J52">
+        <v>6536</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1352</v>
       </c>
@@ -1956,8 +2341,14 @@
       <c r="H53">
         <v>3144</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <v>6484</v>
+      </c>
+      <c r="J53">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1212</v>
       </c>
@@ -1982,8 +2373,14 @@
       <c r="H54">
         <v>1988</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <v>3108</v>
+      </c>
+      <c r="J54">
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1076</v>
       </c>
@@ -2008,8 +2405,14 @@
       <c r="H55">
         <v>1644</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <v>3236</v>
+      </c>
+      <c r="J55">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1076</v>
       </c>
@@ -2034,8 +2437,14 @@
       <c r="H56">
         <v>2760</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <v>3200</v>
+      </c>
+      <c r="J56">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1440</v>
       </c>
@@ -2060,8 +2469,14 @@
       <c r="H57">
         <v>3456</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <v>3196</v>
+      </c>
+      <c r="J57">
+        <v>6016</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>644</v>
       </c>
@@ -2086,8 +2501,14 @@
       <c r="H58">
         <v>1300</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>764</v>
+      </c>
+      <c r="J58">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>912</v>
       </c>
@@ -2112,8 +2533,14 @@
       <c r="H59">
         <v>3000</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <v>1460</v>
+      </c>
+      <c r="J59">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>936</v>
       </c>
@@ -2138,8 +2565,14 @@
       <c r="H60">
         <v>708</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <v>5304</v>
+      </c>
+      <c r="J60">
+        <v>5172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1284</v>
       </c>
@@ -2164,8 +2597,14 @@
       <c r="H61">
         <v>2912</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>6756</v>
+      </c>
+      <c r="J61">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>640</v>
       </c>
@@ -2190,8 +2629,14 @@
       <c r="H62">
         <v>3132</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>11912</v>
+      </c>
+      <c r="J62">
+        <v>7312</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>656</v>
       </c>
@@ -2216,8 +2661,14 @@
       <c r="H63">
         <v>2208</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>2988</v>
+      </c>
+      <c r="J63">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2004</v>
       </c>
@@ -2242,8 +2693,14 @@
       <c r="H64">
         <v>2812</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <v>3008</v>
+      </c>
+      <c r="J64">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>912</v>
       </c>
@@ -2268,8 +2725,14 @@
       <c r="H65">
         <v>6184</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <v>5396</v>
+      </c>
+      <c r="J65">
+        <v>5380</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>708</v>
       </c>
@@ -2294,8 +2757,14 @@
       <c r="H66">
         <v>2100</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66">
+        <v>4528</v>
+      </c>
+      <c r="J66">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>456</v>
       </c>
@@ -2320,8 +2789,14 @@
       <c r="H67">
         <v>4248</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67">
+        <v>3100</v>
+      </c>
+      <c r="J67">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1140</v>
       </c>
@@ -2346,8 +2821,14 @@
       <c r="H68">
         <v>1084</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68">
+        <v>3248</v>
+      </c>
+      <c r="J68">
+        <v>7232</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2020</v>
       </c>
@@ -2372,8 +2853,14 @@
       <c r="H69">
         <v>3124</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>3256</v>
+      </c>
+      <c r="J69">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1044</v>
       </c>
@@ -2398,8 +2885,14 @@
       <c r="H70">
         <v>3216</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>2500</v>
+      </c>
+      <c r="J70">
+        <v>5424</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>632</v>
       </c>
@@ -2424,8 +2917,14 @@
       <c r="H71">
         <v>4704</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <v>6464</v>
+      </c>
+      <c r="J71">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1232</v>
       </c>
@@ -2450,8 +2949,14 @@
       <c r="H72">
         <v>1772</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72">
+        <v>7080</v>
+      </c>
+      <c r="J72">
+        <v>7232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1400</v>
       </c>
@@ -2476,8 +2981,14 @@
       <c r="H73">
         <v>1460</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73">
+        <v>2344</v>
+      </c>
+      <c r="J73">
+        <v>2372</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2344</v>
       </c>
@@ -2502,8 +3013,14 @@
       <c r="H74">
         <v>2756</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74">
+        <v>6324</v>
+      </c>
+      <c r="J74">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2376</v>
       </c>
@@ -2528,8 +3045,14 @@
       <c r="H75">
         <v>6280</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75">
+        <v>5504</v>
+      </c>
+      <c r="J75">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1444</v>
       </c>
@@ -2554,8 +3077,14 @@
       <c r="H76">
         <v>1624</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76">
+        <v>1324</v>
+      </c>
+      <c r="J76">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>672</v>
       </c>
@@ -2580,8 +3109,14 @@
       <c r="H77">
         <v>1748</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77">
+        <v>5356</v>
+      </c>
+      <c r="J77">
+        <v>5420</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1416</v>
       </c>
@@ -2606,8 +3141,14 @@
       <c r="H78">
         <v>516</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78">
+        <v>3096</v>
+      </c>
+      <c r="J78">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1540</v>
       </c>
@@ -2632,8 +3173,14 @@
       <c r="H79">
         <v>2576</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79">
+        <v>3160</v>
+      </c>
+      <c r="J79">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1460</v>
       </c>
@@ -2658,8 +3205,14 @@
       <c r="H80">
         <v>1456</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <v>3064</v>
+      </c>
+      <c r="J80">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>792</v>
       </c>
@@ -2684,8 +3237,14 @@
       <c r="H81">
         <v>1108</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81">
+        <v>6136</v>
+      </c>
+      <c r="J81">
+        <v>7248</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1160</v>
       </c>
@@ -2710,8 +3269,14 @@
       <c r="H82">
         <v>2692</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82">
+        <v>3764</v>
+      </c>
+      <c r="J82">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1296</v>
       </c>
@@ -2736,8 +3301,14 @@
       <c r="H83">
         <v>1360</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <v>5176</v>
+      </c>
+      <c r="J83">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1016</v>
       </c>
@@ -2762,8 +3333,14 @@
       <c r="H84">
         <v>1360</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84">
+        <v>3144</v>
+      </c>
+      <c r="J84">
+        <v>6908</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>716</v>
       </c>
@@ -2788,8 +3365,14 @@
       <c r="H85">
         <v>3120</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85">
+        <v>6884</v>
+      </c>
+      <c r="J85">
+        <v>7048</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1264</v>
       </c>
@@ -2814,8 +3397,14 @@
       <c r="H86">
         <v>3248</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86">
+        <v>10636</v>
+      </c>
+      <c r="J86">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1756</v>
       </c>
@@ -2840,8 +3429,14 @@
       <c r="H87">
         <v>5544</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <v>1016</v>
+      </c>
+      <c r="J87">
+        <v>4916</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>620</v>
       </c>
@@ -2866,8 +3461,14 @@
       <c r="H88">
         <v>3032</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <v>7096</v>
+      </c>
+      <c r="J88">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1036</v>
       </c>
@@ -2892,8 +3493,14 @@
       <c r="H89">
         <v>6656</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89">
+        <v>3240</v>
+      </c>
+      <c r="J89">
+        <v>6056</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>960</v>
       </c>
@@ -2918,8 +3525,14 @@
       <c r="H90">
         <v>1700</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90">
+        <v>2472</v>
+      </c>
+      <c r="J90">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1232</v>
       </c>
@@ -2944,8 +3557,14 @@
       <c r="H91">
         <v>1548</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91">
+        <v>5120</v>
+      </c>
+      <c r="J91">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>340</v>
       </c>
@@ -2970,8 +3589,14 @@
       <c r="H92">
         <v>896</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92">
+        <v>3468</v>
+      </c>
+      <c r="J92">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>704</v>
       </c>
@@ -2996,8 +3621,14 @@
       <c r="H93">
         <v>888</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93">
+        <v>3520</v>
+      </c>
+      <c r="J93">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>680</v>
       </c>
@@ -3022,8 +3653,14 @@
       <c r="H94">
         <v>2620</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94">
+        <v>7332</v>
+      </c>
+      <c r="J94">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>780</v>
       </c>
@@ -3048,8 +3685,14 @@
       <c r="H95">
         <v>2936</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I95">
+        <v>1472</v>
+      </c>
+      <c r="J95">
+        <v>5124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1380</v>
       </c>
@@ -3074,8 +3717,14 @@
       <c r="H96">
         <v>5080</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96">
+        <v>3144</v>
+      </c>
+      <c r="J96">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1428</v>
       </c>
@@ -3100,8 +3749,14 @@
       <c r="H97">
         <v>1212</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97">
+        <v>5660</v>
+      </c>
+      <c r="J97">
+        <v>5204</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1164</v>
       </c>
@@ -3126,8 +3781,14 @@
       <c r="H98">
         <v>2996</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <v>6396</v>
+      </c>
+      <c r="J98">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>644</v>
       </c>
@@ -3152,8 +3813,14 @@
       <c r="H99">
         <v>2732</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99">
+        <v>6928</v>
+      </c>
+      <c r="J99">
+        <v>6632</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1088</v>
       </c>
@@ -3178,8 +3845,14 @@
       <c r="H100">
         <v>2752</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100">
+        <v>6448</v>
+      </c>
+      <c r="J100">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2156</v>
       </c>
@@ -3203,6 +3876,12 @@
       </c>
       <c r="H101">
         <v>3028</v>
+      </c>
+      <c r="I101">
+        <v>3520</v>
+      </c>
+      <c r="J101">
+        <v>1924</v>
       </c>
     </row>
   </sheetData>
@@ -3212,44 +3891,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54DEED1-2593-E04C-A7FC-E90A52BD3EED}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <f>MIN(raw_scores!A2:'raw_scores'!A101)</f>
@@ -3285,12 +3974,16 @@
       </c>
       <c r="J2">
         <f>MIN(raw_scores!I2:'raw_scores'!I101)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>764</v>
+      </c>
+      <c r="K2">
+        <f>MIN(raw_scores!J2:'raw_scores'!J101)</f>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <f>MAX(raw_scores!A2:'raw_scores'!A101)</f>
@@ -3326,12 +4019,16 @@
       </c>
       <c r="J3">
         <f>MAX(raw_scores!I2:'raw_scores'!I101)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11912</v>
+      </c>
+      <c r="K3">
+        <f>MAX(raw_scores!J2:'raw_scores'!J101)</f>
+        <v>7312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <f>AVERAGE(raw_scores!A2:'raw_scores'!A101)</f>
@@ -3365,14 +4062,18 @@
         <f>AVERAGE(raw_scores!H2:'raw_scores'!H101)</f>
         <v>2592</v>
       </c>
-      <c r="J4" t="e">
+      <c r="J4">
         <f>AVERAGE(raw_scores!I2:'raw_scores'!I101)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4312.84</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(raw_scores!J2:'raw_scores'!J101)</f>
+        <v>3675.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <f>MEDIAN(raw_scores!A2:'raw_scores'!A101)</f>
@@ -3406,14 +4107,18 @@
         <f>MEDIAN(raw_scores!H2:'raw_scores'!H101)</f>
         <v>2490</v>
       </c>
-      <c r="J5" t="e">
+      <c r="J5">
         <f>MEDIAN(raw_scores!I2:'raw_scores'!I101)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3568</v>
+      </c>
+      <c r="K5">
+        <f>MEDIAN(raw_scores!J2:'raw_scores'!J101)</f>
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <f>STDEV(raw_scores!A2:'raw_scores'!A101)</f>
@@ -3447,14 +4152,18 @@
         <f>STDEV(raw_scores!H2:'raw_scores'!H101)</f>
         <v>1425.2993731249246</v>
       </c>
-      <c r="J6" t="e">
+      <c r="J6">
         <f>STDEV(raw_scores!I2:'raw_scores'!I101)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2323.3128068307633</v>
+      </c>
+      <c r="K6">
+        <f>STDEV(raw_scores!J2:'raw_scores'!J101)</f>
+        <v>1960.9206079561384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <f>hyper!B2/hyper!B3</f>
@@ -3488,9 +4197,13 @@
         <f>hyper!I2/hyper!I3</f>
         <v>66.98</v>
       </c>
-      <c r="J7" t="e">
+      <c r="J7">
         <f>hyper!J2/hyper!J3</f>
-        <v>#DIV/0!</v>
+        <v>129.47999999999999</v>
+      </c>
+      <c r="K7">
+        <f>hyper!K2/hyper!K3</f>
+        <v>152.13999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>